<commit_message>
update the comments sheet
</commit_message>
<xml_diff>
--- a/mina-mobile-wallet-comments.xlsx
+++ b/mina-mobile-wallet-comments.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\38097\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\coda-mobile-wallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBB8009A-9E30-4305-B2B4-290A13C6F5F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9829C961-6780-483E-928D-55F8DD891884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5907B7A2-299E-447D-B462-CAB15E9F045C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5907B7A2-299E-447D-B462-CAB15E9F045C}"/>
   </bookViews>
   <sheets>
     <sheet name="Designation Challenges" sheetId="1" r:id="rId1"/>
-    <sheet name="Designation Requirements" sheetId="2" r:id="rId2"/>
+    <sheet name="Q&amp;A" sheetId="3" r:id="rId2"/>
+    <sheet name="Designation Requirements" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
   <si>
     <t>Feature</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -494,6 +495,152 @@
         <scheme val="minor"/>
       </rPr>
       <t>", which actually is the operation of undelegation</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I wasn't aware of this. Good catch. I will get back to you on how best to approach this.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I will get back to you on this.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Will resolve based on answers to the above.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>We only need to have one fee. This is an optional feature that gives users choice, similar to this feature in metamask</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agreed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OK we can do this.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>We can get rid of the search field.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Good catch. Agreed.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Also, less savvy crypto holders are often unfamiliar with the term 'delegate'. To simplify things, my idea was to ignore the subtle distinction between staking and delegating, and just call everything staking.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agreed.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>O1lab</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Cata</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>While it's true that tokens can be transferred even if they're staked/delegated, staking returns payouts happen every 30 days, so if you move tokens that you've staked, you'll lose out on all returns you've accrued since your most recent payout (meaning you'll lose out on up to 29 days of returns). 
+For that reason (and others), we don't want staked/delegated tokens to 'feel' available, hence the distinction between staked and available tokens. (Available might not be the best label to use here - I'm open to suggestions). 
+One option is to make no distinction at all - they're all just tokens. But there's definitely a difference between tokens we know you probably don't want to spend (because they're accruing returns), and tokens you know won't accrue returns -- so the display should probably separate those out...though I'm not sure what label to use.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>In MINA you don't have to claim rewards -- they're automatically sent to your staking address. But you're right about 'change pool', we'll need a way to allow users to do that.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(I'm describing the actions of Cardano's Ouroboros protocol, if they are different on this point between Cardano and Mina, please ignore this comment)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Yes the rewards will be deliver to your address automatically from coinbase, then staked automatically. But the rewards can not be spent directly, I must claim them, and then I can transfer them as payment to other users.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(I'm describing the actions of Cardano's Ouroboros protocol, if they are different on this point between Cardano and Mina, please ignore this comment)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+We are clear that the epoch length is two weeks, it should be a little longer depend on the block producing situation and height movement.
+Let's define the current epoch to T0, next T1, third T2, etc.
+How many shares that user have of calculating the chance to produce block depend on the token number on the snapshot of epoch switch. User need not to always hold the tokens.
+Let's have some cases:
+Case 1: User stake his tokens before epoch switch between T0 and T1, and does not cancel his delegation, then he will be rewarded in T2 and the following epoches.
+Case 2: User stake tokens in T0, and cancel delegation before epoch switch between T0 and T1, he will not be rewarded in any epoches.
+Case 3: User stake tokens in T0, and move into T1, but he cancel his delegation before epoch switch between T1 and T2, then he will be rewarded in T2, but lose rewards in the following epoches.
+Case 4: User stake tokens in T0, and move into T2, but he cancel his delegation before epoch switch between T2 and T3, then he will be rewarded in T2, T3, but lose rewards in the following epoches.
+Case 5: User has 100 tokens and stake them in T0, then he send 10 tokens to others before the epoch switch between T0 and T1, then in T2 he will also be rewarded, but the share calculated by 90, not 100. 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>So I think we should be clear the mechanism of mina's protocol, then let's have a further discussion.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -502,7 +649,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,6 +681,23 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -557,7 +721,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -565,6 +729,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -881,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE635400-EA6D-4B01-AD85-22B51CE2027C}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -924,7 +1091,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -939,6 +1106,9 @@
       </c>
       <c r="E2" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="69" x14ac:dyDescent="0.25">
@@ -957,6 +1127,9 @@
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="F3" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="4" spans="1:7" ht="82.8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -974,6 +1147,9 @@
       <c r="E4" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="F4" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -991,8 +1167,11 @@
       <c r="E5" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="F5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="69" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>25</v>
       </c>
@@ -1007,6 +1186,9 @@
       </c>
       <c r="E6" s="1" t="s">
         <v>28</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
@@ -1025,6 +1207,9 @@
       <c r="E7" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="F7" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="8" spans="1:7" ht="69" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -1042,6 +1227,9 @@
       <c r="E8" s="1" t="s">
         <v>37</v>
       </c>
+      <c r="F8" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1059,6 +1247,9 @@
       <c r="E9" s="1" t="s">
         <v>39</v>
       </c>
+      <c r="F9" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1075,6 +1266,20 @@
       </c>
       <c r="E10" s="1" t="s">
         <v>42</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="55.2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1085,6 +1290,55 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EDAA03A-162A-4BF0-A254-CC091035ABCE}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="103.77734375" customWidth="1"/>
+    <col min="2" max="2" width="73" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="23.21875" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="404.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="118.8" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C7F57E-3CF3-43A9-A2A2-37F5E7D7AFDD}">
   <dimension ref="A1:B1"/>
   <sheetViews>

</xml_diff>

<commit_message>
update the wallet comments excel
</commit_message>
<xml_diff>
--- a/mina-mobile-wallet-comments.xlsx
+++ b/mina-mobile-wallet-comments.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\coda-mobile-wallet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9829C961-6780-483E-928D-55F8DD891884}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25561BB0-0EEE-442A-A690-46D83795D566}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{5907B7A2-299E-447D-B462-CAB15E9F045C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5907B7A2-299E-447D-B462-CAB15E9F045C}"/>
   </bookViews>
   <sheets>
     <sheet name="Designation Challenges" sheetId="1" r:id="rId1"/>
-    <sheet name="Q&amp;A" sheetId="3" r:id="rId2"/>
-    <sheet name="Designation Requirements" sheetId="2" r:id="rId3"/>
+    <sheet name="Designation Requirements" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="71">
   <si>
     <t>Feature</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -543,105 +542,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>O1lab</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cata</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>While it's true that tokens can be transferred even if they're staked/delegated, staking returns payouts happen every 30 days, so if you move tokens that you've staked, you'll lose out on all returns you've accrued since your most recent payout (meaning you'll lose out on up to 29 days of returns). 
-For that reason (and others), we don't want staked/delegated tokens to 'feel' available, hence the distinction between staked and available tokens. (Available might not be the best label to use here - I'm open to suggestions). 
-One option is to make no distinction at all - they're all just tokens. But there's definitely a difference between tokens we know you probably don't want to spend (because they're accruing returns), and tokens you know won't accrue returns -- so the display should probably separate those out...though I'm not sure what label to use.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>In MINA you don't have to claim rewards -- they're automatically sent to your staking address. But you're right about 'change pool', we'll need a way to allow users to do that.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(I'm describing the actions of Cardano's Ouroboros protocol, if they are different on this point between Cardano and Mina, please ignore this comment)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Yes the rewards will be deliver to your address automatically from coinbase, then staked automatically. But the rewards can not be spent directly, I must claim them, and then I can transfer them as payment to other users.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(I'm describing the actions of Cardano's Ouroboros protocol, if they are different on this point between Cardano and Mina, please ignore this comment)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-We are clear that the epoch length is two weeks, it should be a little longer depend on the block producing situation and height movement.
-Let's define the current epoch to T0, next T1, third T2, etc.
-How many shares that user have of calculating the chance to produce block depend on the token number on the snapshot of epoch switch. User need not to always hold the tokens.
-Let's have some cases:
-Case 1: User stake his tokens before epoch switch between T0 and T1, and does not cancel his delegation, then he will be rewarded in T2 and the following epoches.
-Case 2: User stake tokens in T0, and cancel delegation before epoch switch between T0 and T1, he will not be rewarded in any epoches.
-Case 3: User stake tokens in T0, and move into T1, but he cancel his delegation before epoch switch between T1 and T2, then he will be rewarded in T2, but lose rewards in the following epoches.
-Case 4: User stake tokens in T0, and move into T2, but he cancel his delegation before epoch switch between T2 and T3, then he will be rewarded in T2, T3, but lose rewards in the following epoches.
-Case 5: User has 100 tokens and stake them in T0, then he send 10 tokens to others before the epoch switch between T0 and T1, then in T2 he will also be rewarded, but the share calculated by 90, not 100. 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>So I think we should be clear the mechanism of mina's protocol, then let's have a further discussion.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="等线"/>
-        <family val="3"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
+    <t>#11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2a. Receive: Multi Account</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Receive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The account seems has alias, but I didn't find how to add alias to account(and this issue exist in other page that show multi account)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The keyboard lack the key "."</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3c. Send: Enter Amount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Backup wallet</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0. Wallet Backup</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I see the mnemonic words when backup and restore wallet, this means we should implement HD wallet(Hierarchical Deterministic Wallet), but it's hard and need lots of research. Even we get it done, the wallet key generated in mobile wallet can not be imported into coda client, so I suggest we manage the keys independently, which as the coda client do now.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -649,7 +594,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -681,23 +626,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF0070C0"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -721,7 +649,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -729,9 +657,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1048,10 +973,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE635400-EA6D-4B01-AD85-22B51CE2027C}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1282,6 +1207,57 @@
         <v>58</v>
       </c>
     </row>
+    <row r="12" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="82.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1290,55 +1266,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EDAA03A-162A-4BF0-A254-CC091035ABCE}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="103.77734375" customWidth="1"/>
-    <col min="2" max="2" width="73" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" customWidth="1"/>
-    <col min="5" max="5" width="23.21875" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="404.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="118.8" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C7F57E-3CF3-43A9-A2A2-37F5E7D7AFDD}">
   <dimension ref="A1:B1"/>
   <sheetViews>

</xml_diff>